<commit_message>
timed mfq functions for various file inputs
</commit_message>
<xml_diff>
--- a/mfq_timings.xlsx
+++ b/mfq_timings.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\megan\Desktop\SpectroMass\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7505E29-D6FD-4F04-9537-C90F83D19A4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FD4126E-0759-48A3-ABBE-07C4E5ABE2FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="timings" sheetId="8" state="hidden" r:id="rId1"/>
-    <sheet name="average graphs" sheetId="4" r:id="rId2"/>
-    <sheet name="function graphs" sheetId="3" r:id="rId3"/>
+    <sheet name="timings" sheetId="8" r:id="rId1"/>
+    <sheet name="average graphs" sheetId="4" state="hidden" r:id="rId2"/>
+    <sheet name="function graphs" sheetId="3" state="hidden" r:id="rId3"/>
     <sheet name="1-15 timings" sheetId="1" r:id="rId4"/>
     <sheet name="864002_Chlamyhistone_CC_G0_1" sheetId="5" r:id="rId5"/>
     <sheet name="863996_Chlamyhistone_CC_G0_2" sheetId="6" r:id="rId6"/>
@@ -344,11 +344,18 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -365,7 +372,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -374,7 +381,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -383,10 +390,31 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -403,34 +431,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -24261,8 +24261,8 @@
   </sheetPr>
   <dimension ref="B1:X87"/>
   <sheetViews>
-    <sheetView topLeftCell="A97" zoomScale="74" zoomScaleNormal="74" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:Q119"/>
+    <sheetView tabSelected="1" zoomScale="74" zoomScaleNormal="74" workbookViewId="0">
+      <selection activeCell="V6" sqref="V6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -24276,15 +24276,15 @@
       <c r="N1" s="9"/>
     </row>
     <row r="2" spans="2:24" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
       <c r="K2" s="10"/>
@@ -24293,27 +24293,27 @@
       <c r="N2" s="4"/>
     </row>
     <row r="3" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
       <c r="L3" s="5"/>
       <c r="M3" s="5"/>
       <c r="N3" s="5"/>
     </row>
     <row r="4" spans="2:24" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
       <c r="I4" s="11"/>
       <c r="J4" s="11"/>
       <c r="K4" s="11"/>
@@ -24322,13 +24322,13 @@
       <c r="N4" s="6"/>
     </row>
     <row r="5" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
       <c r="I5" s="11"/>
       <c r="J5" s="11"/>
       <c r="K5" s="11"/>
@@ -24337,163 +24337,163 @@
       <c r="N5" s="7"/>
     </row>
     <row r="6" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
       <c r="I6" s="11"/>
       <c r="J6" s="11"/>
       <c r="K6" s="11"/>
       <c r="L6" s="11"/>
     </row>
     <row r="7" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
       <c r="I7" s="11"/>
       <c r="J7" s="11"/>
       <c r="K7" s="11"/>
       <c r="L7" s="11"/>
     </row>
     <row r="8" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
     </row>
     <row r="9" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="V9" s="38"/>
-      <c r="W9" s="38"/>
-      <c r="X9" s="38"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="V9" s="14"/>
+      <c r="W9" s="14"/>
+      <c r="X9" s="14"/>
     </row>
     <row r="10" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="V10" s="39"/>
-      <c r="W10" s="39"/>
-      <c r="X10" s="39"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="V10" s="15"/>
+      <c r="W10" s="15"/>
+      <c r="X10" s="15"/>
     </row>
     <row r="11" spans="2:24" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="V11" s="40"/>
-      <c r="W11" s="40"/>
-      <c r="X11" s="40"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="V11" s="16"/>
+      <c r="W11" s="16"/>
+      <c r="X11" s="16"/>
     </row>
     <row r="12" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="V12" s="41"/>
-      <c r="W12" s="41"/>
-      <c r="X12" s="41"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="V12" s="17"/>
+      <c r="W12" s="17"/>
+      <c r="X12" s="17"/>
     </row>
     <row r="13" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="V13" s="42"/>
-      <c r="W13" s="42"/>
-      <c r="X13" s="42"/>
+      <c r="B13" s="20"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
+      <c r="V13" s="18"/>
+      <c r="W13" s="18"/>
+      <c r="X13" s="18"/>
     </row>
     <row r="14" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="B14" s="34"/>
-      <c r="C14" s="34"/>
-      <c r="D14" s="34"/>
-      <c r="E14" s="34"/>
-      <c r="F14" s="17" t="s">
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="G14" s="18"/>
-      <c r="H14" s="19"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="24"/>
     </row>
     <row r="15" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="B15" s="34"/>
-      <c r="C15" s="34"/>
-      <c r="D15" s="34"/>
-      <c r="E15" s="34"/>
-      <c r="F15" s="20" t="s">
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="G15" s="35"/>
-      <c r="H15" s="22"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="27"/>
     </row>
     <row r="16" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="B16" s="34"/>
-      <c r="C16" s="34"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="34"/>
-      <c r="F16" s="23" t="s">
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="G16" s="36"/>
-      <c r="H16" s="25"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="30"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B17" s="34"/>
-      <c r="C17" s="34"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="34"/>
-      <c r="F17" s="26" t="s">
+      <c r="B17" s="19"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="G17" s="37"/>
-      <c r="H17" s="28"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="33"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B18" s="34"/>
-      <c r="C18" s="34"/>
-      <c r="D18" s="34"/>
-      <c r="E18" s="34"/>
-      <c r="F18" s="43" t="s">
+      <c r="B18" s="19"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="G18" s="44"/>
-      <c r="H18" s="45"/>
+      <c r="G18" s="35"/>
+      <c r="H18" s="36"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B19" s="34"/>
-      <c r="C19" s="34"/>
-      <c r="D19" s="34"/>
-      <c r="E19" s="34"/>
-      <c r="F19" s="42"/>
-      <c r="G19" s="42"/>
-      <c r="H19" s="42"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
     </row>
     <row r="73" spans="2:8" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B73" s="13" t="s">
@@ -24507,132 +24507,132 @@
       <c r="H73" s="13"/>
     </row>
     <row r="74" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B74" s="14" t="s">
+      <c r="B74" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="C74" s="14"/>
-      <c r="D74" s="14"/>
-      <c r="E74" s="14"/>
-      <c r="F74" s="14"/>
-      <c r="G74" s="14"/>
-      <c r="H74" s="14"/>
+      <c r="C74" s="20"/>
+      <c r="D74" s="20"/>
+      <c r="E74" s="20"/>
+      <c r="F74" s="20"/>
+      <c r="G74" s="20"/>
+      <c r="H74" s="20"/>
     </row>
     <row r="75" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B75" s="14"/>
-      <c r="C75" s="14"/>
-      <c r="D75" s="14"/>
-      <c r="E75" s="14"/>
-      <c r="F75" s="14"/>
-      <c r="G75" s="14"/>
-      <c r="H75" s="14"/>
+      <c r="B75" s="20"/>
+      <c r="C75" s="20"/>
+      <c r="D75" s="20"/>
+      <c r="E75" s="20"/>
+      <c r="F75" s="20"/>
+      <c r="G75" s="20"/>
+      <c r="H75" s="20"/>
     </row>
     <row r="76" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B76" s="14"/>
-      <c r="C76" s="14"/>
-      <c r="D76" s="14"/>
-      <c r="E76" s="14"/>
-      <c r="F76" s="14"/>
-      <c r="G76" s="14"/>
-      <c r="H76" s="14"/>
+      <c r="B76" s="20"/>
+      <c r="C76" s="20"/>
+      <c r="D76" s="20"/>
+      <c r="E76" s="20"/>
+      <c r="F76" s="20"/>
+      <c r="G76" s="20"/>
+      <c r="H76" s="20"/>
     </row>
     <row r="77" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B77" s="14"/>
-      <c r="C77" s="14"/>
-      <c r="D77" s="14"/>
-      <c r="E77" s="14"/>
-      <c r="F77" s="14"/>
-      <c r="G77" s="14"/>
-      <c r="H77" s="14"/>
+      <c r="B77" s="20"/>
+      <c r="C77" s="20"/>
+      <c r="D77" s="20"/>
+      <c r="E77" s="20"/>
+      <c r="F77" s="20"/>
+      <c r="G77" s="20"/>
+      <c r="H77" s="20"/>
     </row>
     <row r="78" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B78" s="14"/>
-      <c r="C78" s="14"/>
-      <c r="D78" s="14"/>
-      <c r="E78" s="14"/>
-      <c r="F78" s="14"/>
-      <c r="G78" s="14"/>
-      <c r="H78" s="14"/>
+      <c r="B78" s="20"/>
+      <c r="C78" s="20"/>
+      <c r="D78" s="20"/>
+      <c r="E78" s="20"/>
+      <c r="F78" s="20"/>
+      <c r="G78" s="20"/>
+      <c r="H78" s="20"/>
     </row>
     <row r="79" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B79" s="14"/>
-      <c r="C79" s="14"/>
-      <c r="D79" s="14"/>
-      <c r="E79" s="14"/>
-      <c r="F79" s="14"/>
-      <c r="G79" s="14"/>
-      <c r="H79" s="14"/>
+      <c r="B79" s="20"/>
+      <c r="C79" s="20"/>
+      <c r="D79" s="20"/>
+      <c r="E79" s="20"/>
+      <c r="F79" s="20"/>
+      <c r="G79" s="20"/>
+      <c r="H79" s="20"/>
     </row>
     <row r="80" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B80" s="14"/>
-      <c r="C80" s="14"/>
-      <c r="D80" s="14"/>
-      <c r="E80" s="14"/>
-      <c r="F80" s="14"/>
-      <c r="G80" s="14"/>
-      <c r="H80" s="14"/>
+      <c r="B80" s="20"/>
+      <c r="C80" s="20"/>
+      <c r="D80" s="20"/>
+      <c r="E80" s="20"/>
+      <c r="F80" s="20"/>
+      <c r="G80" s="20"/>
+      <c r="H80" s="20"/>
     </row>
     <row r="81" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B81" s="14"/>
-      <c r="C81" s="14"/>
-      <c r="D81" s="14"/>
-      <c r="E81" s="14"/>
-      <c r="F81" s="14"/>
-      <c r="G81" s="14"/>
-      <c r="H81" s="14"/>
+      <c r="B81" s="20"/>
+      <c r="C81" s="20"/>
+      <c r="D81" s="20"/>
+      <c r="E81" s="20"/>
+      <c r="F81" s="20"/>
+      <c r="G81" s="20"/>
+      <c r="H81" s="20"/>
     </row>
     <row r="82" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B82" s="14"/>
-      <c r="C82" s="14"/>
-      <c r="D82" s="14"/>
-      <c r="E82" s="14"/>
-      <c r="F82" s="14"/>
-      <c r="G82" s="14"/>
-      <c r="H82" s="14"/>
+      <c r="B82" s="20"/>
+      <c r="C82" s="20"/>
+      <c r="D82" s="20"/>
+      <c r="E82" s="20"/>
+      <c r="F82" s="20"/>
+      <c r="G82" s="20"/>
+      <c r="H82" s="20"/>
     </row>
     <row r="83" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B83" s="14"/>
-      <c r="C83" s="14"/>
-      <c r="D83" s="14"/>
-      <c r="E83" s="14"/>
-      <c r="F83" s="14"/>
-      <c r="G83" s="14"/>
-      <c r="H83" s="14"/>
+      <c r="B83" s="20"/>
+      <c r="C83" s="20"/>
+      <c r="D83" s="20"/>
+      <c r="E83" s="20"/>
+      <c r="F83" s="20"/>
+      <c r="G83" s="20"/>
+      <c r="H83" s="20"/>
     </row>
     <row r="84" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B84" s="14"/>
-      <c r="C84" s="14"/>
-      <c r="D84" s="14"/>
-      <c r="E84" s="14"/>
-      <c r="F84" s="14"/>
-      <c r="G84" s="14"/>
-      <c r="H84" s="14"/>
+      <c r="B84" s="20"/>
+      <c r="C84" s="20"/>
+      <c r="D84" s="20"/>
+      <c r="E84" s="20"/>
+      <c r="F84" s="20"/>
+      <c r="G84" s="20"/>
+      <c r="H84" s="20"/>
     </row>
     <row r="85" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B85" s="14"/>
-      <c r="C85" s="14"/>
-      <c r="D85" s="14"/>
-      <c r="E85" s="14"/>
-      <c r="F85" s="14"/>
-      <c r="G85" s="14"/>
-      <c r="H85" s="14"/>
+      <c r="B85" s="20"/>
+      <c r="C85" s="20"/>
+      <c r="D85" s="20"/>
+      <c r="E85" s="20"/>
+      <c r="F85" s="20"/>
+      <c r="G85" s="20"/>
+      <c r="H85" s="20"/>
     </row>
     <row r="86" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B86" s="14"/>
-      <c r="C86" s="14"/>
-      <c r="D86" s="14"/>
-      <c r="E86" s="14"/>
-      <c r="F86" s="14"/>
-      <c r="G86" s="14"/>
-      <c r="H86" s="14"/>
+      <c r="B86" s="20"/>
+      <c r="C86" s="20"/>
+      <c r="D86" s="20"/>
+      <c r="E86" s="20"/>
+      <c r="F86" s="20"/>
+      <c r="G86" s="20"/>
+      <c r="H86" s="20"/>
     </row>
     <row r="87" spans="2:8" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B87" s="14"/>
-      <c r="C87" s="14"/>
-      <c r="D87" s="14"/>
-      <c r="E87" s="14"/>
-      <c r="F87" s="14"/>
-      <c r="G87" s="14"/>
-      <c r="H87" s="14"/>
+      <c r="B87" s="20"/>
+      <c r="C87" s="20"/>
+      <c r="D87" s="20"/>
+      <c r="E87" s="20"/>
+      <c r="F87" s="20"/>
+      <c r="G87" s="20"/>
+      <c r="H87" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -24656,7 +24656,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B7F51C7-4000-4D9F-AE03-35E19716E15A}">
   <dimension ref="B1:N19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+    <sheetView zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:H3"/>
     </sheetView>
   </sheetViews>
@@ -24671,15 +24671,15 @@
       <c r="N1" s="9"/>
     </row>
     <row r="2" spans="2:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
       <c r="K2" s="10"/>
@@ -24688,27 +24688,27 @@
       <c r="N2" s="4"/>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
       <c r="L3" s="5"/>
       <c r="M3" s="5"/>
       <c r="N3" s="5"/>
     </row>
     <row r="4" spans="2:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
       <c r="I4" s="11"/>
       <c r="J4" s="11"/>
       <c r="K4" s="11"/>
@@ -24717,13 +24717,13 @@
       <c r="N4" s="6"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
       <c r="I5" s="11"/>
       <c r="J5" s="11"/>
       <c r="K5" s="11"/>
@@ -24732,48 +24732,48 @@
       <c r="N5" s="7"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
       <c r="I6" s="11"/>
       <c r="J6" s="11"/>
       <c r="K6" s="11"/>
       <c r="L6" s="11"/>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
       <c r="I7" s="11"/>
       <c r="J7" s="11"/>
       <c r="K7" s="11"/>
       <c r="L7" s="11"/>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B10" s="11"/>
@@ -24785,92 +24785,92 @@
       <c r="H10" s="11"/>
     </row>
     <row r="11" spans="2:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
       <c r="E11" s="11"/>
-      <c r="F11" s="17" t="s">
+      <c r="F11" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="G11" s="18"/>
-      <c r="H11" s="19"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="24"/>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
       <c r="E12" s="11"/>
-      <c r="F12" s="20" t="s">
+      <c r="F12" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="G12" s="21"/>
-      <c r="H12" s="22"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="27"/>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
+      <c r="B13" s="20"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
       <c r="E13" s="11"/>
-      <c r="F13" s="23" t="s">
+      <c r="F13" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="G13" s="24"/>
-      <c r="H13" s="25"/>
+      <c r="G13" s="39"/>
+      <c r="H13" s="30"/>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="F14" s="26" t="s">
+      <c r="B14" s="20"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="F14" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="G14" s="27"/>
-      <c r="H14" s="28"/>
+      <c r="G14" s="40"/>
+      <c r="H14" s="33"/>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="F15" s="29" t="s">
+      <c r="B15" s="20"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="F15" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="G15" s="30"/>
-      <c r="H15" s="31"/>
+      <c r="G15" s="42"/>
+      <c r="H15" s="43"/>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="F16" s="32"/>
-      <c r="G16" s="32"/>
-      <c r="H16" s="32"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="F16" s="44"/>
+      <c r="G16" s="44"/>
+      <c r="H16" s="44"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="F19" s="15"/>
-      <c r="G19" s="15"/>
-      <c r="H19" s="15"/>
+      <c r="F19" s="37"/>
+      <c r="G19" s="37"/>
+      <c r="H19" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -24903,143 +24903,143 @@
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="2" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
     </row>
     <row r="4" spans="2:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
+      <c r="B13" s="20"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
+      <c r="B14" s="20"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>